<commit_message>
UML Merge & Modify Actor Descripition
</commit_message>
<xml_diff>
--- a/SE_16_B711084_배형민.xlsx
+++ b/SE_16_B711084_배형민.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="87">
   <si>
     <t xml:space="preserve"> Requirement list  (functional, non-functional 구분)</t>
   </si>
@@ -82,31 +82,22 @@
     <t>description</t>
   </si>
   <si>
-    <t>고객</t>
-  </si>
-  <si>
-    <t>고객은 회원정보를 입력하여 회원가입을 할 수 있습니다.</t>
-  </si>
-  <si>
     <t>회원</t>
   </si>
   <si>
-    <t>회원은 로그인을 통해 시스템에 대한 사용 권한을 얻을 수 있습니다.</t>
-  </si>
-  <si>
-    <t>고객(판매자)</t>
-  </si>
-  <si>
-    <t>판매자는 의류를 등록, 판매, 조회, 수정 할 수 있습니다.</t>
-  </si>
-  <si>
-    <t>고객(구매자)</t>
+    <t>회원은 회원가입을 할 수 있고, 로그인을 통해 시스템에 대한 사용 권한을 얻을 수 있습니다. 또한 로그인 하여 의류를 등록/ 판매/ 조회 할 수 있습니다.</t>
+  </si>
+  <si>
+    <t>프로그램 종료</t>
+  </si>
+  <si>
+    <t>회원이 로그아웃 시 자동으로 프로그램을 종료합니다.</t>
+  </si>
+  <si>
+    <t>택배사</t>
   </si>
   <si>
     <t>...</t>
-  </si>
-  <si>
-    <t>택배사</t>
   </si>
   <si>
     <t>이메일</t>
@@ -815,38 +806,20 @@
       <c r="E14" s="14"/>
     </row>
     <row r="15">
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" s="14"/>
-    </row>
-    <row r="16">
-      <c r="C16" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="14"/>
-    </row>
-    <row r="17">
-      <c r="C17" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E17" s="15"/>
+      <c r="D15" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="15"/>
     </row>
     <row r="28">
       <c r="A28" s="1">
         <v>3.0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34">
@@ -854,13 +827,13 @@
         <v>4.0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E34" s="18"/>
     </row>
@@ -869,7 +842,7 @@
         <v>5</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E35" s="14"/>
     </row>
@@ -878,7 +851,7 @@
         <v>7</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E36" s="14"/>
     </row>
@@ -887,7 +860,7 @@
         <v>9</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E37" s="14"/>
     </row>
@@ -896,7 +869,7 @@
         <v>11</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E38" s="14"/>
     </row>
@@ -905,7 +878,7 @@
         <v>13</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E39" s="14"/>
     </row>
@@ -914,7 +887,7 @@
         <v>15</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E40" s="14"/>
     </row>
@@ -923,7 +896,7 @@
         <v>17</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E41" s="14"/>
     </row>
@@ -932,7 +905,7 @@
         <v>19</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E42" s="15"/>
     </row>
@@ -943,37 +916,37 @@
     </row>
     <row r="46">
       <c r="C46" s="16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D46" s="17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E46" s="18"/>
     </row>
     <row r="47">
       <c r="C47" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E47" s="14"/>
     </row>
     <row r="48">
       <c r="C48" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E48" s="14"/>
     </row>
     <row r="49">
       <c r="C49" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E49" s="15"/>
     </row>
@@ -984,47 +957,47 @@
     </row>
     <row r="52">
       <c r="C52" s="16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D52" s="17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="53">
       <c r="C53" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54">
       <c r="C54" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55">
       <c r="C55" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="56">
       <c r="C56" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="57">
       <c r="C57" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="59">
@@ -1034,26 +1007,26 @@
     </row>
     <row r="60">
       <c r="C60" s="16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D60" s="17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="61">
       <c r="C61" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="62">
       <c r="C62" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="64">
@@ -1063,142 +1036,142 @@
     </row>
     <row r="65">
       <c r="C65" s="16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D65" s="17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="66">
       <c r="C66" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="67">
       <c r="C67" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="69">
       <c r="C69" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="70">
       <c r="C70" s="16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D70" s="17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="71">
       <c r="C71" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="72">
       <c r="C72" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="73">
       <c r="C73" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="74">
       <c r="C74" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="76">
       <c r="C76" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="77">
       <c r="C77" s="16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D77" s="17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="78">
       <c r="C78" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="79">
       <c r="C79" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="81">
       <c r="C81" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="82">
       <c r="C82" s="16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D82" s="17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="83">
       <c r="C83" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="84">
       <c r="C84" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="85">
       <c r="C85" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="86">
       <c r="C86" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="88">
@@ -1208,42 +1181,42 @@
     </row>
     <row r="89">
       <c r="C89" s="16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D89" s="17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="90">
       <c r="C90" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="91">
       <c r="C91" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="92">
       <c r="C92" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="93">
       <c r="C93" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>